<commit_message>
Inserção da classe Disciplina.py
</commit_message>
<xml_diff>
--- a/Docs/EsbocoDiagramaClasses.xlsx
+++ b/Docs/EsbocoDiagramaClasses.xlsx
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="135">
   <si>
     <t>Data</t>
   </si>
@@ -1335,10 +1335,16 @@
     </r>
   </si>
   <si>
-    <t>Materia</t>
-  </si>
-  <si>
     <t>Professor</t>
+  </si>
+  <si>
+    <t>Disciplina</t>
+  </si>
+  <si>
+    <t>nota</t>
+  </si>
+  <si>
+    <t>Nota</t>
   </si>
 </sst>
 </file>
@@ -1463,14 +1469,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1484,10 +1484,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1784,8 +1791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1810,865 +1817,866 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="13"/>
+      <c r="D1" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="G1" s="2" t="s">
+      <c r="E1" s="13"/>
+      <c r="G1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="2" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="2" t="s">
+      <c r="K1" s="13"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="13"/>
       <c r="P1" s="14" t="s">
         <v>117</v>
       </c>
       <c r="Q1" s="14"/>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="T1" s="2"/>
+      <c r="T1" s="13"/>
       <c r="V1" s="14" t="s">
         <v>65</v>
       </c>
       <c r="W1" s="14"/>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="Z1" s="2"/>
-      <c r="AB1" s="1" t="s">
+      <c r="Z1" s="13"/>
+      <c r="AB1" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="AC1" s="15"/>
+      <c r="AE1" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="AF1" s="15"/>
+      <c r="AH1" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="AC1" s="1"/>
-      <c r="AE1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="AF1" s="1"/>
-      <c r="AH1" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="AI1" s="1"/>
+      <c r="AI1" s="15"/>
     </row>
     <row r="2" spans="1:35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="3" t="s">
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="3" t="s">
+      <c r="K2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="3" t="s">
+      <c r="N2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="S2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="V2" s="15" t="s">
+      <c r="T2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="W2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y2" s="3" t="s">
+      <c r="W2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="Z2" s="9" t="s">
+      <c r="Z2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:35">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="3" t="s">
+      <c r="H3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="11"/>
+      <c r="J3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M3" s="3" t="s">
+      <c r="K3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P3" s="3" t="s">
+      <c r="N3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="9" t="s">
+      <c r="T3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="V3" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="W3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y3" s="3" t="s">
+      <c r="W3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="Z3" s="9" t="s">
+      <c r="Z3" s="7" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:35">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="13"/>
-      <c r="J4" s="3" t="s">
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="3" t="s">
+      <c r="K4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P4" s="3" t="s">
+      <c r="N4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Q4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="S4" s="3" t="s">
+      <c r="Q4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="T4" s="9" t="s">
+      <c r="T4" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="V4" s="15" t="s">
+      <c r="V4" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="W4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y4" s="3" t="s">
+      <c r="W4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y4" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="Z4" s="9" t="s">
+      <c r="Z4" s="7" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:35">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="7" t="s">
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="3" t="s">
+      <c r="H5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="11"/>
+      <c r="J5" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="3" t="s">
+      <c r="K5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="N5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P5" s="5" t="s">
+      <c r="N5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="Q5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="S5" s="3" t="s">
+      <c r="Q5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="T5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="V5" s="15" t="s">
+      <c r="T5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V5" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="W5" s="9" t="s">
+      <c r="W5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Y5" s="3" t="s">
+      <c r="Y5" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="Z5" s="7" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="5" t="s">
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="13"/>
-      <c r="J6" s="3" t="s">
+      <c r="H6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="11"/>
+      <c r="J6" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="K6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M6" s="5" t="s">
+      <c r="K6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="N6" s="6"/>
-      <c r="P6" s="5" t="s">
+      <c r="N6" s="4"/>
+      <c r="P6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="6"/>
-      <c r="S6" s="3" t="s">
+      <c r="Q6" s="4"/>
+      <c r="S6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="T6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="V6" s="15" t="s">
+      <c r="T6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="V6" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="W6" s="9" t="s">
+      <c r="W6" s="7" t="s">
         <v>70</v>
       </c>
       <c r="Y6" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="Z6" s="11" t="s">
-        <v>20</v>
+        <v>133</v>
+      </c>
+      <c r="Z6" s="16" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:35">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="B7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="3" t="s">
+      <c r="H7" s="4"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" s="5" t="s">
+      <c r="K7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="N7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P7" s="5" t="s">
+      <c r="N7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P7" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="Q7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="S7" s="3" t="s">
+      <c r="Q7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="T7" s="9" t="s">
+      <c r="T7" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="V7" s="5" t="s">
+      <c r="V7" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="W7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y7" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z7" s="11" t="s">
-        <v>117</v>
+      <c r="W7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z7" s="9" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:35">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="B8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="5" t="s">
+      <c r="E8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="13"/>
-      <c r="J8" s="3" t="s">
+      <c r="H8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M8" s="5" t="s">
+      <c r="K8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="N8" s="6"/>
-      <c r="P8" s="5" t="s">
+      <c r="N8" s="4"/>
+      <c r="P8" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="Q8" s="6"/>
-      <c r="S8" s="5" t="s">
+      <c r="Q8" s="4"/>
+      <c r="S8" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="T8" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="V8" s="5" t="s">
+      <c r="T8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="V8" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="W8" s="6"/>
-      <c r="Y8" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z8" s="11" t="s">
-        <v>118</v>
+      <c r="W8" s="4"/>
+      <c r="Y8" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z8" s="9" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:35">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="D9" s="5" t="s">
+      <c r="B9" s="4"/>
+      <c r="D9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="G9" s="5" t="s">
+      <c r="E9" s="4"/>
+      <c r="G9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="3" t="s">
+      <c r="H9" s="4"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="K9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M9" s="5" t="s">
+      <c r="K9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="N9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P9" s="5" t="s">
+      <c r="N9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="Q9" s="6" t="s">
+      <c r="Q9" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="S9" s="5" t="s">
+      <c r="S9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="T9" s="6"/>
-      <c r="V9" s="5" t="s">
+      <c r="T9" s="4"/>
+      <c r="V9" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="W9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y9" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="Z9" s="11" t="s">
-        <v>105</v>
+      <c r="W9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z9" s="9" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:35">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="5" t="s">
+      <c r="E10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I10" s="13"/>
-      <c r="J10" s="3" t="s">
+      <c r="H10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="K10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M10" s="5" t="s">
+      <c r="K10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="N10" s="6"/>
-      <c r="P10" s="5" t="s">
+      <c r="N10" s="4"/>
+      <c r="P10" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="Q10" s="6" t="s">
+      <c r="Q10" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="S10" s="5" t="s">
+      <c r="S10" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="T10" s="11" t="s">
+      <c r="T10" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="V10" s="5" t="s">
+      <c r="V10" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="W10" s="6"/>
+      <c r="W10" s="4"/>
+      <c r="Y10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z10" s="9" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="11" spans="1:35">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="D11" s="5" t="s">
+      <c r="B11" s="4"/>
+      <c r="D11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="G11" s="5" t="s">
+      <c r="E11" s="4"/>
+      <c r="G11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="5" t="s">
+      <c r="H11" s="4"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P11" s="5" t="s">
+      <c r="K11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="P11" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="Q11" s="6" t="s">
+      <c r="Q11" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="S11" s="5" t="s">
+      <c r="S11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="T11" s="11" t="s">
+      <c r="T11" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="V11" s="5" t="s">
+      <c r="V11" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="W11" s="6" t="s">
+      <c r="W11" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:35">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="5" t="s">
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="5" t="s">
+      <c r="E12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I12" s="13"/>
-      <c r="J12" s="5" t="s">
+      <c r="H12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="K12" s="6"/>
-      <c r="S12" s="5" t="s">
+      <c r="K12" s="4"/>
+      <c r="S12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="T12" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="V12" s="5" t="s">
+      <c r="T12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="V12" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="W12" s="6"/>
+      <c r="W12" s="4"/>
     </row>
     <row r="13" spans="1:35">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="D13" s="5" t="s">
+      <c r="B13" s="4"/>
+      <c r="D13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="G13" s="5" t="s">
+      <c r="E13" s="4"/>
+      <c r="G13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="5" t="s">
+      <c r="H13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="11"/>
+      <c r="J13" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="K13" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="S13" s="5" t="s">
+      <c r="K13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S13" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="T13" s="6"/>
-      <c r="V13" s="5" t="s">
+      <c r="T13" s="4"/>
+      <c r="V13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="W13" s="11" t="s">
+      <c r="W13" s="9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:35">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="B14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="5" t="s">
+      <c r="E14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="6"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="5" t="s">
+      <c r="H14" s="4"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="K14" s="6"/>
-      <c r="S14" s="5" t="s">
+      <c r="K14" s="4"/>
+      <c r="S14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="T14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="V14" s="5" t="s">
+      <c r="T14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="V14" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="W14" s="11" t="s">
+      <c r="W14" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:35">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="D15" s="5" t="s">
+      <c r="B15" s="4"/>
+      <c r="D15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="6"/>
-      <c r="J15" s="5" t="s">
+      <c r="E15" s="4"/>
+      <c r="J15" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="K15" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="S15" s="5" t="s">
+      <c r="K15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="T15" s="6"/>
+      <c r="T15" s="4"/>
     </row>
     <row r="16" spans="1:35">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="5" t="s">
+      <c r="B16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" s="5" t="s">
+      <c r="E16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="K16" s="6"/>
-      <c r="S16" s="5" t="s">
+      <c r="K16" s="4"/>
+      <c r="S16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="T16" s="6" t="s">
+      <c r="T16" s="4" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:20">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="D17" s="5" t="s">
+      <c r="B17" s="4"/>
+      <c r="D17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="J17" s="5" t="s">
+      <c r="E17" s="4"/>
+      <c r="J17" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="K17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="S17" s="5" t="s">
+      <c r="K17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="S17" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="T17" s="6" t="s">
+      <c r="T17" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:20">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="5" t="s">
+      <c r="B18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="E18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="K18" s="6"/>
-      <c r="S18" s="5" t="s">
+      <c r="K18" s="4"/>
+      <c r="S18" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="T18" s="6" t="s">
+      <c r="T18" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:20">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="J19" s="5" t="s">
+      <c r="B19" s="4"/>
+      <c r="J19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="K19" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:20">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J20" s="5" t="s">
+      <c r="B20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="K20" s="6"/>
+      <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:20">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J21" s="5" t="s">
+      <c r="B21" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="K21" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:20">
-      <c r="J22" s="5" t="s">
+      <c r="J22" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="K22" s="6"/>
+      <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:20">
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="K23" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:20">
-      <c r="J24" s="5" t="s">
+      <c r="J24" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="K24" s="6"/>
+      <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:20">
-      <c r="J25" s="5" t="s">
+      <c r="J25" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K25" s="6" t="s">
+      <c r="K25" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:20">
-      <c r="J26" s="5" t="s">
+      <c r="J26" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="K26" s="6"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:20">
-      <c r="J27" s="5" t="s">
+      <c r="J27" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="K27" s="6" t="s">
+      <c r="K27" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:20">
-      <c r="J28" s="5" t="s">
+      <c r="J28" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="K28" s="6"/>
+      <c r="K28" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="S1:T1"/>
@@ -2676,6 +2684,11 @@
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="V1:W1"/>
     <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AE1:AF1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adicionado Aluno.py e Editado EsbocoDiagramaClasses.xlsx
</commit_message>
<xml_diff>
--- a/Docs/EsbocoDiagramaClasses.xlsx
+++ b/Docs/EsbocoDiagramaClasses.xlsx
@@ -1096,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+    <sheetView tabSelected="1" topLeftCell="J11" workbookViewId="0">
+      <selection activeCell="S29" sqref="S28:S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1784,7 +1784,7 @@
         <v>134</v>
       </c>
       <c r="N17" s="6" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="P17" s="11" t="s">
         <v>80</v>
@@ -2037,7 +2037,7 @@
         <v>137</v>
       </c>
       <c r="N24" s="22" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="P24" s="9" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Inserção de Data.py Ja configurada no BD
</commit_message>
<xml_diff>
--- a/Docs/EsbocoDiagramaClasses.xlsx
+++ b/Docs/EsbocoDiagramaClasses.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="6855" yWindow="-120" windowWidth="11115" windowHeight="6855"/>
@@ -11,12 +11,12 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="151">
   <si>
     <t>Data</t>
   </si>
@@ -30,12 +30,6 @@
     <t>hora</t>
   </si>
   <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t>seg</t>
-  </si>
-  <si>
     <t>str</t>
   </si>
   <si>
@@ -54,12 +48,6 @@
     <t>getHora()</t>
   </si>
   <si>
-    <t>getMin()</t>
-  </si>
-  <si>
-    <t>getSeg()</t>
-  </si>
-  <si>
     <t>DadosPessoais</t>
   </si>
   <si>
@@ -180,12 +168,6 @@
     <t>setHora(novoHora)</t>
   </si>
   <si>
-    <t>setMin(novoMin)</t>
-  </si>
-  <si>
-    <t>setSeg(novoSeg)</t>
-  </si>
-  <si>
     <t>setId(novoId)</t>
   </si>
   <si>
@@ -484,6 +466,9 @@
   </si>
   <si>
     <t>excluirDisc(id)</t>
+  </si>
+  <si>
+    <t>addNova(ano, mes, dia, hora)</t>
   </si>
 </sst>
 </file>
@@ -537,7 +522,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -750,6 +735,17 @@
       <bottom style="dotted">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -774,20 +770,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,6 +795,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1094,10 +1090,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T52"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J11" workbookViewId="0">
-      <selection activeCell="S29" sqref="S28:S29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1129,80 +1125,80 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="D1" s="25" t="s">
+      <c r="B1" s="27"/>
+      <c r="D1" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="25"/>
+      <c r="G1" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="25"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="25"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="25"/>
+      <c r="P1" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q1" s="25"/>
+      <c r="S1" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="G1" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="25" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" s="26"/>
-      <c r="P1" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="Q1" s="26"/>
-      <c r="S1" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="T1" s="26"/>
+      <c r="T1" s="25"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:20">
@@ -1210,89 +1206,89 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="Q3" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="S3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S4" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:20">
@@ -1300,44 +1296,44 @@
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:20">
@@ -1345,1107 +1341,1071 @@
         <v>3</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E6" s="12"/>
       <c r="G6" s="9" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="N6" s="12"/>
       <c r="P6" s="7" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>6</v>
+      <c r="A7" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="2"/>
       <c r="J7" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="K7" s="10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P7" s="9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q7" s="10" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="S7" s="11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="T7" s="12"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>6</v>
-      </c>
+      <c r="A8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="12"/>
       <c r="D8" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E8" s="12"/>
       <c r="G8" s="11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="K8" s="12"/>
       <c r="M8" s="11" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="N8" s="12"/>
       <c r="P8" s="11" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="Q8" s="12"/>
       <c r="S8" s="11" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="T8" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>48</v>
+      <c r="A9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="2"/>
       <c r="J9" s="11" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="M9" s="11" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P9" s="11" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="S9" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="T9" s="12"/>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="11" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B10" s="12"/>
       <c r="D10" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="11" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="K10" s="12"/>
       <c r="M10" s="11" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="N10" s="12"/>
       <c r="P10" s="11" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="Q10" s="12"/>
       <c r="S10" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="T10" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="2"/>
       <c r="J11" s="11" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M11" s="11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P11" s="11" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="S11" s="11" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="T11" s="12"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B12" s="12"/>
-      <c r="D12" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>34</v>
+      <c r="D12" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="11" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="K12" s="12"/>
       <c r="M12" s="13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="N12" s="14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P12" s="11" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="Q12" s="12"/>
       <c r="S12" s="11" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="2"/>
       <c r="J13" s="11" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="P13" s="11" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="S13" s="11" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="T13" s="12"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B14" s="12"/>
       <c r="G14" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="H14" s="17" t="s">
-        <v>34</v>
+        <v>122</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="11" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="K14" s="12"/>
-      <c r="M14" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="N14" s="26"/>
+      <c r="M14" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" s="25"/>
       <c r="P14" s="11" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="Q14" s="12"/>
       <c r="S14" s="11" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="26"/>
+        <v>4</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="25"/>
       <c r="G15" s="13" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="K15" s="12" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P15" s="11" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="Q15" s="12" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="S15" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="T15" s="17" t="s">
-        <v>34</v>
+        <v>74</v>
+      </c>
+      <c r="T15" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B16" s="12"/>
       <c r="D16" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="K16" s="12"/>
       <c r="M16" s="5" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="N16" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="P16" s="11" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="Q16" s="12"/>
       <c r="S16" s="13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="T16" s="14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>6</v>
+        <v>150</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" s="25"/>
+      <c r="J17" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P17" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q17" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="J18" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="H17" s="26"/>
-      <c r="J17" s="18" t="s">
+      <c r="K18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="P18" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q18" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="S18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="S19" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="T19" s="25"/>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="D20" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="K20" s="25"/>
+      <c r="M20" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="N20" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="P20" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q20" s="25"/>
+      <c r="S20" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="D21" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="M21" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="N21" s="19"/>
+      <c r="P21" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="S21" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="T21" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="H22" s="19"/>
+      <c r="J22" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="N22" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q22" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M23" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="K17" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P17" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q17" s="12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="12"/>
-      <c r="D18" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="3" t="s">
+      <c r="N23" s="19"/>
+      <c r="P23" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q23" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="G24" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H24" s="16"/>
+      <c r="J24" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="J18" s="13" t="s">
+      <c r="K24" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M24" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="N24" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q24" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="K18" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="M18" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P18" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q18" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="S18" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="S19" s="25" t="s">
-        <v>151</v>
-      </c>
-      <c r="T19" s="26"/>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="A20" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="12"/>
-      <c r="D20" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="H20" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J20" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="K20" s="26"/>
-      <c r="M20" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="N20" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="P20" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q20" s="26"/>
-      <c r="S20" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="T20" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20">
-      <c r="A21" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="H25" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="K25" s="19"/>
+      <c r="M25" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="N25" s="19"/>
+      <c r="P25" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q25" s="19"/>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="16"/>
+      <c r="G26" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="H26" s="16"/>
+      <c r="J26" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="M26" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="N26" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="P26" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q26" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="H21" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="M21" s="21" t="s">
-        <v>136</v>
-      </c>
-      <c r="N21" s="22"/>
-      <c r="P21" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="Q21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="S21" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="T21" s="24" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="A22" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="D22" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="G22" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="H22" s="22"/>
-      <c r="J22" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="K22" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M22" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="N22" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="P22" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q22" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20">
-      <c r="A23" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G23" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="H23" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="M23" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="N23" s="22"/>
-      <c r="P23" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q23" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20">
-      <c r="A24" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" s="17"/>
-      <c r="G24" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="H24" s="17"/>
-      <c r="J24" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="K24" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="M24" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="N24" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="P24" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q24" s="10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
-      <c r="D25" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="G25" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="H25" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J25" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="K25" s="22"/>
-      <c r="M25" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="N25" s="22"/>
-      <c r="P25" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q25" s="22"/>
-    </row>
-    <row r="26" spans="1:20">
-      <c r="A26" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B26" s="20"/>
-      <c r="D26" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="E26" s="17"/>
-      <c r="G26" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="H26" s="17"/>
-      <c r="J26" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="M26" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="N26" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="P26" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q26" s="17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20">
-      <c r="A27" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>34</v>
+      <c r="H27" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="K27" s="17"/>
-      <c r="M27" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="N27" s="22"/>
+        <v>104</v>
+      </c>
+      <c r="K27" s="16"/>
+      <c r="M27" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="N27" s="19"/>
       <c r="P27" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q27" s="17"/>
+        <v>104</v>
+      </c>
+      <c r="Q27" s="16"/>
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="5" t="s">
         <v>24</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D28" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" s="16"/>
+      <c r="G28" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="M28" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="N28" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="P28" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q28" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="K29" s="16"/>
+      <c r="M29" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="N29" s="19"/>
+      <c r="P29" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q29" s="16"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="16"/>
+      <c r="J30" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="M30" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="N30" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="P30" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q30" s="16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="D31" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="K31" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="M31" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="N31" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="P31" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q31" s="14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="16"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="D33" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="G28" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="K28" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="M28" s="21" t="s">
-        <v>139</v>
-      </c>
-      <c r="N28" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="P28" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="Q28" s="17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20">
-      <c r="A29" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" s="11" t="s">
+      <c r="E34" s="16"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="12"/>
+      <c r="D35" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E29" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J29" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="K29" s="17"/>
-      <c r="M29" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="N29" s="22"/>
-      <c r="P29" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q29" s="17"/>
-    </row>
-    <row r="30" spans="1:20">
-      <c r="A30" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="17"/>
-      <c r="J30" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="K30" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="M30" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="N30" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="P30" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q30" s="17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20">
-      <c r="A31" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J31" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="K31" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="M31" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="N31" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="P31" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q31" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20">
-      <c r="A32" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E32" s="17"/>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="E34" s="17"/>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>48</v>
+      <c r="E35" s="16" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" s="12"/>
+        <v>27</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="D36" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="E36" s="17"/>
+        <v>84</v>
+      </c>
+      <c r="E36" s="16"/>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>34</v>
+        <v>55</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="D37" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="12"/>
+        <v>28</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>4</v>
+      </c>
       <c r="D38" s="13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>48</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B39" s="12"/>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B40" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>6</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="B41" s="12"/>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B42" s="12"/>
+        <v>29</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="12" t="s">
-        <v>6</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B43" s="12"/>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B44" s="12"/>
+        <v>59</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>6</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B45" s="12"/>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" s="12"/>
+      <c r="A46" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B48" s="12"/>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B50" s="12"/>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="B51" s="17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="B52" s="14" t="s">
-        <v>34</v>
+      <c r="A47" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD FUNCOES LOGIN EM BANCO DE DADOS E ADD CLASSE Login.py FUNCIONANDO OK COM O BANCO
</commit_message>
<xml_diff>
--- a/Docs/EsbocoDiagramaClasses.xlsx
+++ b/Docs/EsbocoDiagramaClasses.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="153">
   <si>
     <t>Data</t>
   </si>
@@ -469,6 +469,12 @@
   </si>
   <si>
     <t>addNova(ano, mes, dia, hora)</t>
+  </si>
+  <si>
+    <t>getSenha()</t>
+  </si>
+  <si>
+    <t>setSenha(novoSenha)</t>
   </si>
 </sst>
 </file>
@@ -752,7 +758,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -789,13 +795,20 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1093,7 +1106,7 @@
   <dimension ref="A1:T47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1125,36 +1138,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="D1" s="24" t="s">
+      <c r="B1" s="30"/>
+      <c r="D1" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="G1" s="24" t="s">
+      <c r="E1" s="28"/>
+      <c r="G1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="25"/>
+      <c r="H1" s="28"/>
       <c r="I1" s="2"/>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="25"/>
+      <c r="K1" s="28"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="25"/>
-      <c r="P1" s="24" t="s">
+      <c r="N1" s="28"/>
+      <c r="P1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="Q1" s="25"/>
-      <c r="S1" s="24" t="s">
+      <c r="Q1" s="28"/>
+      <c r="S1" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="T1" s="25"/>
+      <c r="T1" s="28"/>
     </row>
     <row r="2" spans="1:20">
       <c r="A2" s="3" t="s">
@@ -1460,10 +1473,10 @@
       <c r="B9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="12" t="s">
+      <c r="D9" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="31" t="s">
         <v>4</v>
       </c>
       <c r="G9" s="11" t="s">
@@ -1500,11 +1513,9 @@
       </c>
       <c r="B10" s="12"/>
       <c r="D10" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>4</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="E10" s="12"/>
       <c r="G10" s="11" t="s">
         <v>90</v>
       </c>
@@ -1539,10 +1550,10 @@
         <v>4</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>91</v>
@@ -1577,11 +1588,11 @@
         <v>46</v>
       </c>
       <c r="B12" s="12"/>
-      <c r="D12" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>30</v>
+      <c r="D12" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>83</v>
@@ -1618,10 +1629,10 @@
       <c r="B13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="E13" s="14" t="s">
+      <c r="D13" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>30</v>
       </c>
       <c r="G13" s="11" t="s">
@@ -1651,6 +1662,12 @@
         <v>48</v>
       </c>
       <c r="B14" s="12"/>
+      <c r="D14" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>30</v>
+      </c>
       <c r="G14" s="11" t="s">
         <v>122</v>
       </c>
@@ -1662,10 +1679,10 @@
         <v>117</v>
       </c>
       <c r="K14" s="12"/>
-      <c r="M14" s="24" t="s">
+      <c r="M14" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="N14" s="25"/>
+      <c r="N14" s="28"/>
       <c r="P14" s="11" t="s">
         <v>117</v>
       </c>
@@ -1684,10 +1701,12 @@
       <c r="B15" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="25"/>
+      <c r="D15" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="G15" s="13" t="s">
         <v>99</v>
       </c>
@@ -1724,12 +1743,6 @@
         <v>49</v>
       </c>
       <c r="B16" s="12"/>
-      <c r="D16" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>4</v>
-      </c>
       <c r="J16" s="11" t="s">
         <v>119</v>
       </c>
@@ -1755,19 +1768,17 @@
       <c r="A17" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="24" t="s">
+      <c r="B17" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="25"/>
+      <c r="G17" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="H17" s="25"/>
+      <c r="H17" s="28"/>
       <c r="J17" s="17" t="s">
         <v>98</v>
       </c>
@@ -1794,10 +1805,10 @@
       <c r="B18" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="D18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G18" s="3" t="s">
@@ -1836,10 +1847,10 @@
         <v>30</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>94</v>
@@ -1853,14 +1864,14 @@
       <c r="N19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="S19" s="24" t="s">
+      <c r="S19" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="T19" s="25"/>
+      <c r="T19" s="28"/>
     </row>
     <row r="20" spans="1:20">
       <c r="D20" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>4</v>
@@ -1871,20 +1882,20 @@
       <c r="H20" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="24" t="s">
+      <c r="J20" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="K20" s="25"/>
+      <c r="K20" s="28"/>
       <c r="M20" s="9" t="s">
         <v>129</v>
       </c>
       <c r="N20" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="P20" s="24" t="s">
+      <c r="P20" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="Q20" s="25"/>
+      <c r="Q20" s="28"/>
       <c r="S20" s="3" t="s">
         <v>146</v>
       </c>
@@ -1898,10 +1909,10 @@
       </c>
       <c r="B21" s="23"/>
       <c r="D21" s="5" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G21" s="9" t="s">
         <v>47</v>
@@ -1939,11 +1950,11 @@
       <c r="B22" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>44</v>
+      <c r="D22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="G22" s="18" t="s">
         <v>50</v>
@@ -1975,10 +1986,10 @@
       <c r="B23" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="10" t="s">
+      <c r="D23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="6" t="s">
         <v>4</v>
       </c>
       <c r="G23" s="11" t="s">
@@ -2011,10 +2022,12 @@
       <c r="B24" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="16"/>
+      <c r="D24" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>44</v>
+      </c>
       <c r="G24" s="11" t="s">
         <v>104</v>
       </c>
@@ -2045,11 +2058,11 @@
       <c r="B25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>44</v>
+      <c r="D25" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>105</v>
@@ -2078,7 +2091,7 @@
         <v>4</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="E26" s="16"/>
       <c r="G26" s="11" t="s">
@@ -2111,11 +2124,11 @@
       <c r="B27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="17" t="s">
-        <v>75</v>
+      <c r="D27" s="11" t="s">
+        <v>73</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="G27" s="11" t="s">
         <v>74</v>
@@ -2144,7 +2157,7 @@
         <v>4</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="E28" s="16"/>
       <c r="G28" s="13" t="s">
@@ -2179,8 +2192,8 @@
       <c r="B29" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="11" t="s">
-        <v>77</v>
+      <c r="D29" s="17" t="s">
+        <v>75</v>
       </c>
       <c r="E29" s="16" t="s">
         <v>4</v>
@@ -2206,7 +2219,7 @@
         <v>44</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E30" s="16"/>
       <c r="J30" s="11" t="s">
@@ -2234,7 +2247,7 @@
       </c>
       <c r="B31" s="12"/>
       <c r="D31" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E31" s="16" t="s">
         <v>4</v>
@@ -2265,8 +2278,8 @@
       <c r="B32" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D32" s="17" t="s">
-        <v>80</v>
+      <c r="D32" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="E32" s="16"/>
     </row>
@@ -2276,7 +2289,7 @@
       </c>
       <c r="B33" s="12"/>
       <c r="D33" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E33" s="16" t="s">
         <v>4</v>
@@ -2289,8 +2302,8 @@
       <c r="B34" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="11" t="s">
-        <v>82</v>
+      <c r="D34" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="E34" s="16"/>
     </row>
@@ -2300,10 +2313,10 @@
       </c>
       <c r="B35" s="12"/>
       <c r="D35" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>44</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -2314,7 +2327,7 @@
         <v>4</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E36" s="16"/>
     </row>
@@ -2323,11 +2336,11 @@
         <v>55</v>
       </c>
       <c r="B37" s="12"/>
-      <c r="D37" s="17" t="s">
-        <v>96</v>
+      <c r="D37" s="11" t="s">
+        <v>83</v>
       </c>
       <c r="E37" s="16" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -2337,18 +2350,22 @@
       <c r="B38" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>30</v>
-      </c>
+      <c r="D38" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38" s="16"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="11" t="s">
         <v>56</v>
       </c>
       <c r="B39" s="12"/>
+      <c r="D39" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="11" t="s">
@@ -2357,6 +2374,12 @@
       <c r="B40" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="D40" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="11" t="s">
@@ -2409,7 +2432,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="M14:N14"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="P20:Q20"/>
@@ -2421,7 +2444,6 @@
     <mergeCell ref="J20:K20"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="G17:H17"/>
-    <mergeCell ref="D15:E15"/>
     <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>